<commit_message>
Added columns to clean
</commit_message>
<xml_diff>
--- a/tidy_metadata.xlsx
+++ b/tidy_metadata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t xml:space="preserve">col_names</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t xml:space="preserve">biopsy_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_authors_annotation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">disease_subtype</t>
   </si>
 </sst>
 </file>
@@ -496,6 +505,22 @@
         <v>14</v>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
tidy metadata now independent for capital letter and punctuation
</commit_message>
<xml_diff>
--- a/tidy_metadata.xlsx
+++ b/tidy_metadata.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t xml:space="preserve">col_names</t>
   </si>
@@ -20,27 +20,21 @@
     <t xml:space="preserve">general</t>
   </si>
   <si>
-    <t xml:space="preserve">patient.id</t>
+    <t xml:space="preserve">patient_id</t>
   </si>
   <si>
     <t xml:space="preserve">patient</t>
   </si>
   <si>
-    <t xml:space="preserve">patient_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">donor</t>
   </si>
   <si>
-    <t xml:space="preserve">sample.id</t>
+    <t xml:space="preserve">sample_id</t>
   </si>
   <si>
     <t xml:space="preserve">sample</t>
   </si>
   <si>
-    <t xml:space="preserve">sample_id</t>
-  </si>
-  <si>
     <t xml:space="preserve">response</t>
   </si>
   <si>
@@ -59,9 +53,6 @@
     <t xml:space="preserve">biopsy</t>
   </si>
   <si>
-    <t xml:space="preserve">biopsy.id</t>
-  </si>
-  <si>
     <t xml:space="preserve">biopsy_location</t>
   </si>
   <si>
@@ -78,6 +69,12 @@
   </si>
   <si>
     <t xml:space="preserve">disease_subtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cell_subtype</t>
+  </si>
+  <si>
+    <t xml:space="preserve">annotation_authors_minor</t>
   </si>
 </sst>
 </file>
@@ -438,87 +435,71 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="s">
         <v>20</v>
-      </c>
-      <c r="B14" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>